<commit_message>
RPA-112: 4-18 varsel yngre enn 15 dgr
</commit_message>
<xml_diff>
--- a/Vasklister/Excel/vaskeliste_v2.0.xlsx
+++ b/Vasklister/Excel/vaskeliste_v2.0.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5996" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5993" uniqueCount="30">
   <si>
     <t>debitor_ident</t>
   </si>
@@ -100,19 +100,10 @@
     <t>FJELLHAMAR</t>
   </si>
   <si>
-    <t>984661185</t>
+    <t>8 333,33</t>
   </si>
   <si>
-    <t>POSTEN NORGE AS</t>
-  </si>
-  <si>
-    <t>Lørenskogveien 50_x000D_</t>
-  </si>
-  <si>
-    <t>1470 LØRENSKOG_x000D_</t>
-  </si>
-  <si>
-    <t>8 333,33</t>
+    <t>A-Inntekt Failed</t>
   </si>
 </sst>
 </file>
@@ -458,8 +449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T300"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AB3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -468,7 +459,8 @@
     <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.42578125" style="1"/>
+    <col min="6" max="6" width="11.42578125" style="1"/>
+    <col min="7" max="7" width="22.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="12" width="11.42578125" style="1"/>
     <col min="13" max="13" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -551,7 +543,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>23</v>
@@ -577,17 +569,8 @@
       <c r="L2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
@@ -19068,5 +19051,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>